<commit_message>
final data and code
</commit_message>
<xml_diff>
--- a/Compiled_experiment_data.xlsx
+++ b/Compiled_experiment_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbenjamin/Desktop/McMaster/Synchrony/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED46EBE-04CB-2B43-A125-4371814A7CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551CB082-CC7C-1F48-AA0B-FB6CDD1D24DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13420" xr2:uid="{BAD7D914-73E3-4243-B7D9-FB7210C6BDCF}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AL$44</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1147,8 +1147,8 @@
   <dimension ref="A1:AL145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U10" sqref="U10"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>